<commit_message>
changes WDS csv and updated flow changes
</commit_message>
<xml_diff>
--- a/UCG/WDS/DataDocs/WDSLOAD-V1-Articles.xlsx
+++ b/UCG/WDS/DataDocs/WDSLOAD-V1-Articles.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2840" yWindow="3580" windowWidth="29840" windowHeight="16040" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="16520" yWindow="580" windowWidth="51940" windowHeight="17720" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="69">
   <si>
     <t>Query</t>
   </si>
@@ -157,9 +157,6 @@
     <t>Credit Card Stolen? Here's What You Do</t>
   </si>
   <si>
-    <t>What should I do if my credit card is stolen?</t>
-  </si>
-  <si>
     <t>Preventive measures to take against Fraud</t>
   </si>
   <si>
@@ -170,15 +167,6 @@
   </si>
   <si>
     <t>Financial liability due to stolen credit cards</t>
-  </si>
-  <si>
-    <t>What is my liability due to a stolen credit card?</t>
-  </si>
-  <si>
-    <t>What preventitive measure can I take due to credit card loss?</t>
-  </si>
-  <si>
-    <t>I am a victim of credit fraud?</t>
   </si>
   <si>
     <t>What-is-covered-by-basic-Auto-Insurance-Policy</t>
@@ -277,6 +265,21 @@
   </si>
   <si>
     <t>What is an adjustable rate mortgage</t>
+  </si>
+  <si>
+    <t>I am a victim of fraud?</t>
+  </si>
+  <si>
+    <t>What should I do if my card is stolen?</t>
+  </si>
+  <si>
+    <t>What is my liability due to a stolen card?</t>
+  </si>
+  <si>
+    <t>What is my liability due to fraud?</t>
+  </si>
+  <si>
+    <t>What preventitive measure can I take due to losing a card?</t>
   </si>
 </sst>
 </file>
@@ -753,7 +756,7 @@
     </row>
     <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -768,7 +771,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
@@ -834,7 +837,7 @@
     </row>
     <row r="22" spans="1:1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -847,12 +850,12 @@
     </row>
     <row r="25" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A25" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="26" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
@@ -865,12 +868,12 @@
     </row>
     <row r="29" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A29" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
@@ -883,12 +886,12 @@
     </row>
     <row r="33" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A33" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
@@ -901,12 +904,12 @@
     </row>
     <row r="37" spans="1:1" s="19" customFormat="1" ht="20" x14ac:dyDescent="0.2">
       <c r="A37" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="26" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
@@ -919,17 +922,17 @@
     </row>
     <row r="41" spans="1:1" s="19" customFormat="1" ht="20" x14ac:dyDescent="0.2">
       <c r="A41" s="27" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="22" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="18" x14ac:dyDescent="0.2">
@@ -1815,8 +1818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2378,10 +2381,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2447,7 +2450,7 @@
         <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C2" s="4">
         <v>100</v>
@@ -2465,13 +2468,13 @@
         <v>80</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I2" s="4">
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="K2" s="4">
         <v>0</v>
@@ -2488,7 +2491,7 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C3" s="4">
         <v>100</v>
@@ -2506,13 +2509,13 @@
         <v>80</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="I3" s="4">
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="K3" s="4">
         <v>0</v>
@@ -2529,7 +2532,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C4" s="4">
         <v>100</v>
@@ -2547,13 +2550,13 @@
         <v>80</v>
       </c>
       <c r="H4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I4" s="4">
         <v>0</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K4" s="4">
         <v>0</v>
@@ -2570,7 +2573,7 @@
         <v>25</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C5" s="7">
         <v>100</v>
@@ -2588,13 +2591,13 @@
         <v>80</v>
       </c>
       <c r="H5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I5" s="4">
         <v>0</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K5" s="7">
         <v>0</v>
@@ -2611,7 +2614,7 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C6" s="7">
         <v>100</v>
@@ -2629,13 +2632,13 @@
         <v>80</v>
       </c>
       <c r="H6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I6" s="4">
         <v>0</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K6" s="7">
         <v>0</v>
@@ -2649,10 +2652,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C7" s="4">
         <v>100</v>
@@ -2690,10 +2693,10 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C8" s="4">
         <v>100</v>
@@ -2731,10 +2734,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C9" s="4">
         <v>100</v>
@@ -2772,22 +2775,22 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C10" s="4">
         <v>100</v>
       </c>
-      <c r="D10" t="s">
-        <v>53</v>
+      <c r="D10" s="13" t="s">
+        <v>13</v>
       </c>
       <c r="E10" s="4">
         <v>90</v>
       </c>
-      <c r="F10" t="s">
-        <v>52</v>
+      <c r="F10" s="13" t="s">
+        <v>13</v>
       </c>
       <c r="G10" s="4">
         <v>80</v>
@@ -2812,52 +2815,52 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="4">
+        <v>100</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="4">
+        <v>90</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="4">
+        <v>80</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="24">
-        <v>100</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="24">
-        <v>90</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="24">
-        <v>80</v>
-      </c>
-      <c r="H11" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="I11" s="24">
-        <v>0</v>
-      </c>
-      <c r="J11" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="K11" s="24">
-        <v>0</v>
-      </c>
-      <c r="L11" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="M11" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" t="s">
-        <v>65</v>
+      <c r="B12" s="23" t="s">
+        <v>42</v>
       </c>
       <c r="C12" s="24">
         <v>100</v>
@@ -2874,31 +2877,31 @@
       <c r="G12" s="24">
         <v>80</v>
       </c>
-      <c r="H12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="4">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" s="4">
-        <v>0</v>
-      </c>
-      <c r="L12" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="M12" s="4">
+      <c r="H12" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="24">
+        <v>0</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="K12" s="24">
+        <v>0</v>
+      </c>
+      <c r="L12" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="M12" s="24">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C13" s="24">
         <v>100</v>
@@ -2931,6 +2934,47 @@
         <v>13</v>
       </c>
       <c r="M13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="24">
+        <v>100</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="24">
+        <v>90</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="24">
+        <v>80</v>
+      </c>
+      <c r="H14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" s="4">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
daily changes - nothing special
</commit_message>
<xml_diff>
--- a/UCG/WDS/DataDocs/WDSLOAD-V1-Articles.xlsx
+++ b/UCG/WDS/DataDocs/WDSLOAD-V1-Articles.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16520" yWindow="580" windowWidth="51940" windowHeight="17720" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="19520" yWindow="8040" windowWidth="51940" windowHeight="17720" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="66">
   <si>
     <t>Query</t>
   </si>
@@ -256,15 +256,6 @@
   </si>
   <si>
     <t>HOW DOES AN ARM WORK</t>
-  </si>
-  <si>
-    <t>HOW-DOES-AN-ARM-WORK</t>
-  </si>
-  <si>
-    <t>What is an ARM</t>
-  </si>
-  <si>
-    <t>What is an adjustable rate mortgage</t>
   </si>
   <si>
     <t>I am a victim of fraud?</t>
@@ -2381,10 +2372,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2652,7 +2643,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
         <v>47</v>
@@ -2693,7 +2684,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
         <v>48</v>
@@ -2734,7 +2725,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
         <v>49</v>
@@ -2775,7 +2766,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
         <v>48</v>
@@ -2816,7 +2807,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
         <v>50</v>
@@ -2893,88 +2884,6 @@
         <v>13</v>
       </c>
       <c r="M12" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="24">
-        <v>100</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="24">
-        <v>90</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="24">
-        <v>80</v>
-      </c>
-      <c r="H13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="4">
-        <v>0</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="4">
-        <v>0</v>
-      </c>
-      <c r="L13" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="M13" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="24">
-        <v>100</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="24">
-        <v>90</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="24">
-        <v>80</v>
-      </c>
-      <c r="H14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="4">
-        <v>0</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K14" s="4">
-        <v>0</v>
-      </c>
-      <c r="L14" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="M14" s="4">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated flows files from dev cluster to rep
</commit_message>
<xml_diff>
--- a/UCG/WDS/DataDocs/WDSLOAD-V1-Articles.xlsx
+++ b/UCG/WDS/DataDocs/WDSLOAD-V1-Articles.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19520" yWindow="8040" windowWidth="51940" windowHeight="17720" tabRatio="500" activeTab="2"/>
+    <workbookView minimized="1" xWindow="0" yWindow="9760" windowWidth="33600" windowHeight="17720" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -204,12 +204,6 @@
 Other factors varying among states include the cost and frequency of litigation; medical care and repair costs; prevalence of auto insurance fraud; and weather trends.</t>
   </si>
   <si>
-    <t>Life insurance premiums depend on the age of the insured party. Because younger people are less likely to die than older people, younger people typically pay lower life insurance costs. Gender plays a similar role. Because women tend to live longer than men, women tend to pay lower premiums. Engaging in risky activities increases insurance costs. 
-For example, a racecar driver faces increased risk of death and, as a result, may pay high life insurance premiums or be denied coverage.  A person's medical records help determine insurance rates. A history of chronic disease or other potential health issues with an individual or family, such as heart disease or cancer, may result in paying higher premiums. 
-Obesity, alcohol consumption or smoking can affect rates as well. An applicant typically goes through a medical exam to determine whether he has high blood pressure or other signs of potential health issues that may result in premature death for the applicant and increased risk for the insurance company. People in good health typically pay lower life insurance premiums.  
-A person pays more for insurance coverage for a longer policy term and a larger death benefit. For example, the risk of dying for a person with a 30-year policy is greater than the risk of dying for a person with a 10-year policy.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Contact one of the three major credit bureaus, Equifax (888-766-0008), Experian (888-397-3742) or TransUnion (800-680-7289), and place an Initial Fraud Alert on your credit file for 90 days if you suspect you have been, or are about to be, a victim of identity theft. Whichever bureau you contact will notify the other two to do the same. If you wish, you can renew these fraud alerts each quarter, free of charge.  
 If you determine that you actually have suffered identity theft, you can also file an Extended Fraud Alert, which will stay on your reports for seven years. To do so, you’ll need to submit an Identity Theft Report, as outlined below.  Placing a fraud alert entitles you to one free credit report from each bureau. 
 Although the alert makes it harder for someone to open new credit accounts in your name, it won’t necessarily prevent them from using existing accounts. That’s why it’s important to close compromised accounts and to carefully review your credit reports for errors, fraudulent activity or suspicious credit inquiries from an unfamiliar source. 
@@ -271,6 +265,12 @@
   </si>
   <si>
     <t>What preventitive measure can I take due to losing a card?</t>
+  </si>
+  <si>
+    <t>Life insurance premiums depend on the age of the insured party. Because younger people are less likely to die than older people, younger people typically pay lower life insurance costs. Gender plays a similar role. Because women tend to live longer than men, women tend to pay lower premiums. Engaging in risky activities increases insurance costs. 
+For example, a race car driver faces increased risk of death and, as a result, may pay high life insurance premiums or be denied coverage.  A person's medical records help determine insurance rates. A history of chronic disease or other potential health issues with an individual or family, such as heart disease or cancer, may result in paying higher premiums. 
+Obesity, alcohol consumption or smoking can affect rates as well. An applicant typically goes through a medical exam to determine whether he has high blood pressure or other signs of potential health issues that may result in premature death for the applicant and increased risk for the insurance company. People in good health typically pay lower life insurance premiums.  
+A person pays more for insurance coverage for a longer policy term and a larger death benefit. For example, the risk of dying for a person with a 30-year policy is greater than the risk of dying for a person with a 10-year policy.</t>
   </si>
 </sst>
 </file>
@@ -732,7 +732,7 @@
   <dimension ref="A1:A622"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -762,7 +762,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
@@ -828,7 +828,7 @@
     </row>
     <row r="22" spans="1:1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -846,7 +846,7 @@
     </row>
     <row r="26" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
@@ -864,7 +864,7 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
@@ -882,7 +882,7 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
@@ -900,7 +900,7 @@
     </row>
     <row r="38" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
@@ -913,12 +913,12 @@
     </row>
     <row r="41" spans="1:1" s="19" customFormat="1" ht="20" x14ac:dyDescent="0.2">
       <c r="A41" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="16" x14ac:dyDescent="0.2">
@@ -1809,8 +1809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1875,7 +1875,7 @@
       </c>
       <c r="B3" s="17" t="str">
         <f ca="1">TRIM(OFFSET(Data!$A3,(ROW()-2)*3,0))</f>
-        <v>Life insurance premiums depend on the age of the insured party. Because younger people are less likely to die than older people, younger people typically pay lower life insurance costs. Gender plays a similar role. Because women tend to live longer than men, women tend to pay lower premiums. Engaging in risky activities increases insurance costs. _x000D__x000D_For example, a racecar driver faces increased risk of death and, as a result, may pay high life insurance premiums or be denied coverage. A person's medical records help determine insurance rates. A history of chronic disease or other potential health issues with an individual or family, such as heart disease or cancer, may result in paying higher premiums. _x000D__x000D_Obesity, alcohol consumption or smoking can affect rates as well. An applicant typically goes through a medical exam to determine whether he has high blood pressure or other signs of potential health issues that may result in premature death for the applicant and increased risk for the insurance company. People in good health typically pay lower life insurance premiums. _x000D__x000D_A person pays more for insurance coverage for a longer policy term and a larger death benefit. For example, the risk of dying for a person with a 30-year policy is greater than the risk of dying for a person with a 10-year policy.</v>
+        <v>Life insurance premiums depend on the age of the insured party. Because younger people are less likely to die than older people, younger people typically pay lower life insurance costs. Gender plays a similar role. Because women tend to live longer than men, women tend to pay lower premiums. Engaging in risky activities increases insurance costs. _x000D__x000D_For example, a race car driver faces increased risk of death and, as a result, may pay high life insurance premiums or be denied coverage. A person's medical records help determine insurance rates. A history of chronic disease or other potential health issues with an individual or family, such as heart disease or cancer, may result in paying higher premiums. _x000D__x000D_Obesity, alcohol consumption or smoking can affect rates as well. An applicant typically goes through a medical exam to determine whether he has high blood pressure or other signs of potential health issues that may result in premature death for the applicant and increased risk for the insurance company. People in good health typically pay lower life insurance premiums. _x000D__x000D_A person pays more for insurance coverage for a longer policy term and a larger death benefit. For example, the risk of dying for a person with a 30-year policy is greater than the risk of dying for a person with a 10-year policy.</v>
       </c>
       <c r="C3" s="5" t="str">
         <f ca="1">TRIM(OFFSET(Data!$A4,(ROW()-2)*3,0))</f>
@@ -2375,7 +2375,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2643,7 +2643,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
         <v>47</v>
@@ -2684,7 +2684,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
         <v>48</v>
@@ -2725,7 +2725,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
         <v>49</v>
@@ -2766,7 +2766,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
         <v>48</v>
@@ -2807,7 +2807,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
         <v>50</v>

</xml_diff>